<commit_message>
Se han agregado varias bebidas
</commit_message>
<xml_diff>
--- a/POSvNova_1.xlsx
+++ b/POSvNova_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="POS" sheetId="3" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="COMPRAS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="329">
   <si>
     <t>Codigo</t>
   </si>
@@ -943,6 +942,69 @@
   </si>
   <si>
     <t>cervesa vintoria 1,2L</t>
+  </si>
+  <si>
+    <t>7501055305629</t>
+  </si>
+  <si>
+    <t>742097352081</t>
+  </si>
+  <si>
+    <t>9002490100070</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Sprite 600ml</t>
+  </si>
+  <si>
+    <t>7501055303793</t>
+  </si>
+  <si>
+    <t>Lift 600ml</t>
+  </si>
+  <si>
+    <t>7501055300952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca Cola 1.25L </t>
+  </si>
+  <si>
+    <t>Red Bull 250ml</t>
+  </si>
+  <si>
+    <t>742097352029</t>
+  </si>
+  <si>
+    <t>742097352043</t>
+  </si>
+  <si>
+    <t>742097352074</t>
+  </si>
+  <si>
+    <t>742097352036</t>
+  </si>
+  <si>
+    <t>Fersan manzanita 500ml</t>
+  </si>
+  <si>
+    <t>Fersan naranja 500ml</t>
+  </si>
+  <si>
+    <t>Fersan fresa 500ml</t>
+  </si>
+  <si>
+    <t>Fersan toronja 500ml</t>
+  </si>
+  <si>
+    <t>742097352067</t>
+  </si>
+  <si>
+    <t>Fersan durazno 500ml</t>
+  </si>
+  <si>
+    <t>Fersan piña 500ml</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1067,6 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,7 +1394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1341,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F501"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -1368,7 +1431,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7"/>
-      <c r="B2" s="19" t="str">
+      <c r="B2" s="28" t="str">
         <f>IFERROR(VLOOKUP($A2,DB!$A$2:$D$503,2,FALSE),"")</f>
         <v/>
       </c>
@@ -1462,7 +1525,9 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>311</v>
+      </c>
       <c r="B10" s="19" t="str">
         <f>IFERROR(VLOOKUP($A10,DB!$A$2:$D$503,2,FALSE),"")</f>
         <v/>
@@ -6911,10 +6976,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F616"/>
+  <dimension ref="A1:H616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7642,7 +7707,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:8">
       <c r="A49" s="9" t="s">
         <v>109</v>
       </c>
@@ -7657,7 +7722,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:8">
       <c r="A50" s="9" t="s">
         <v>111</v>
       </c>
@@ -7672,7 +7737,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:8">
       <c r="A51" s="9" t="s">
         <v>114</v>
       </c>
@@ -7687,7 +7752,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:8">
       <c r="A52" s="9" t="s">
         <v>105</v>
       </c>
@@ -7702,7 +7767,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:8">
       <c r="A53" s="9" t="s">
         <v>117</v>
       </c>
@@ -7717,7 +7782,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:8">
       <c r="A54" s="9" t="s">
         <v>119</v>
       </c>
@@ -7732,7 +7797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:8">
       <c r="A55" s="9" t="s">
         <v>121</v>
       </c>
@@ -7747,7 +7812,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:8">
       <c r="A56" s="9" t="s">
         <v>122</v>
       </c>
@@ -7762,7 +7827,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:8">
       <c r="A57" s="9" t="s">
         <v>125</v>
       </c>
@@ -7776,8 +7841,18 @@
       <c r="E57" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>90.5</v>
+      </c>
+      <c r="G57">
+        <v>12</v>
+      </c>
+      <c r="H57">
+        <f>F57/G57</f>
+        <v>7.541666666666667</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="9" t="s">
         <v>127</v>
       </c>
@@ -7792,7 +7867,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:8">
       <c r="A59" s="9" t="s">
         <v>129</v>
       </c>
@@ -7807,7 +7882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60" s="9" t="s">
         <v>131</v>
       </c>
@@ -7822,7 +7897,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:8">
       <c r="A61" s="9" t="s">
         <v>133</v>
       </c>
@@ -7837,7 +7912,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:8">
       <c r="A62" s="9" t="s">
         <v>136</v>
       </c>
@@ -7852,7 +7927,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:8">
       <c r="A63" s="9" t="s">
         <v>139</v>
       </c>
@@ -7867,7 +7942,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:8">
       <c r="A64" s="9" t="s">
         <v>141</v>
       </c>
@@ -8840,7 +8915,7 @@
       </c>
       <c r="E128" s="8"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:7">
       <c r="A129" s="9" t="s">
         <v>283</v>
       </c>
@@ -8853,7 +8928,7 @@
       </c>
       <c r="E129" s="8"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:7">
       <c r="A130" s="9" t="s">
         <v>286</v>
       </c>
@@ -8866,7 +8941,7 @@
       </c>
       <c r="E130" s="8"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:7">
       <c r="A131" s="9" t="s">
         <v>306</v>
       </c>
@@ -8879,79 +8954,176 @@
       </c>
       <c r="E131" s="8"/>
     </row>
-    <row r="132" spans="1:5">
-      <c r="B132" s="18"/>
+    <row r="132" spans="1:7">
+      <c r="A132" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>312</v>
+      </c>
       <c r="C132" s="18"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="8"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="B133" s="18"/>
+      <c r="D132" s="2">
+        <v>9</v>
+      </c>
+      <c r="E132" s="8">
+        <v>84.5</v>
+      </c>
+      <c r="F132">
+        <v>12</v>
+      </c>
+      <c r="G132">
+        <f>E132/F132</f>
+        <v>7.041666666666667</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>314</v>
+      </c>
       <c r="C133" s="18"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="8"/>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="B134" s="18"/>
+      <c r="D133" s="2">
+        <v>9</v>
+      </c>
+      <c r="E133" s="8">
+        <v>84.5</v>
+      </c>
+      <c r="F133">
+        <v>12</v>
+      </c>
+      <c r="G133">
+        <f>E133/F133</f>
+        <v>7.041666666666667</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>316</v>
+      </c>
       <c r="C134" s="18"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="8"/>
-    </row>
-    <row r="135" spans="1:5">
-      <c r="B135" s="18"/>
+      <c r="D134" s="2">
+        <v>14</v>
+      </c>
+      <c r="E134" s="8">
+        <v>92</v>
+      </c>
+      <c r="F134">
+        <v>8</v>
+      </c>
+      <c r="G134">
+        <f>E134/F134</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B135" s="18" t="s">
+        <v>317</v>
+      </c>
       <c r="C135" s="18"/>
-      <c r="D135" s="2"/>
+      <c r="D135" s="2">
+        <v>30</v>
+      </c>
       <c r="E135" s="8"/>
     </row>
-    <row r="136" spans="1:5">
-      <c r="B136" s="18"/>
+    <row r="136" spans="1:7">
+      <c r="A136" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="B136" s="18" t="s">
+        <v>324</v>
+      </c>
       <c r="C136" s="18"/>
-      <c r="D136" s="2"/>
+      <c r="D136" s="2">
+        <v>5</v>
+      </c>
       <c r="E136" s="8"/>
     </row>
-    <row r="137" spans="1:5">
-      <c r="B137" s="18"/>
+    <row r="137" spans="1:7">
+      <c r="A137" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B137" s="18" t="s">
+        <v>323</v>
+      </c>
       <c r="C137" s="18"/>
-      <c r="D137" s="2"/>
+      <c r="D137" s="2">
+        <v>5</v>
+      </c>
       <c r="E137" s="8"/>
     </row>
-    <row r="138" spans="1:5">
-      <c r="B138" s="18"/>
+    <row r="138" spans="1:7">
+      <c r="A138" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>322</v>
+      </c>
       <c r="C138" s="18"/>
-      <c r="D138" s="2"/>
+      <c r="D138" s="2">
+        <v>5</v>
+      </c>
       <c r="E138" s="8"/>
     </row>
-    <row r="139" spans="1:5">
-      <c r="B139" s="18"/>
+    <row r="139" spans="1:7">
+      <c r="A139" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B139" s="18" t="s">
+        <v>325</v>
+      </c>
       <c r="C139" s="18"/>
-      <c r="D139" s="2"/>
+      <c r="D139" s="2">
+        <v>5</v>
+      </c>
       <c r="E139" s="8"/>
     </row>
-    <row r="140" spans="1:5">
-      <c r="B140" s="18"/>
+    <row r="140" spans="1:7">
+      <c r="A140" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B140" s="18" t="s">
+        <v>327</v>
+      </c>
       <c r="C140" s="18"/>
-      <c r="D140" s="2"/>
+      <c r="D140" s="2">
+        <v>5</v>
+      </c>
       <c r="E140" s="8"/>
     </row>
-    <row r="141" spans="1:5">
-      <c r="B141" s="18"/>
+    <row r="141" spans="1:7">
+      <c r="A141" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B141" s="18" t="s">
+        <v>328</v>
+      </c>
       <c r="C141" s="18"/>
-      <c r="D141" s="2"/>
+      <c r="D141" s="2">
+        <v>5</v>
+      </c>
       <c r="E141" s="8"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:7">
       <c r="B142" s="18"/>
       <c r="C142" s="18"/>
       <c r="D142" s="2"/>
       <c r="E142" s="8"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:7">
       <c r="B143" s="18"/>
       <c r="C143" s="18"/>
       <c r="D143" s="2"/>
       <c r="E143" s="8"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:7">
       <c r="B144" s="18"/>
       <c r="C144" s="18"/>
       <c r="D144" s="2"/>
@@ -11799,7 +11971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>

</xml_diff>